<commit_message>
updated plotting code for stage two to include variables that aren't in stage one
</commit_message>
<xml_diff>
--- a/data_visualization/stages_check/name_mapping_DSM.xlsx
+++ b/data_visualization/stages_check/name_mapping_DSM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sara/Code/MLABcode/data_visualization/stages_check/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6798FAD-93D1-F640-8D4A-DA79B1635EFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{855816B3-DBD3-CD46-AB44-92AF9E385922}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{B31395B6-E6C3-3F47-A9CB-556FD15C08CD}"/>
+    <workbookView xWindow="35140" yWindow="2380" windowWidth="28800" windowHeight="17500" xr2:uid="{B31395B6-E6C3-3F47-A9CB-556FD15C08CD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1044,8 +1044,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{500C0A2A-D934-4445-A24A-031F5F468C93}">
   <dimension ref="A1:T995"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="B139" sqref="B139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5582,8 +5582,12 @@
       <c r="B140" s="2"/>
       <c r="C140" s="1"/>
       <c r="D140" s="1"/>
-      <c r="E140" s="1"/>
-      <c r="F140" s="1"/>
+      <c r="E140" s="1">
+        <v>1</v>
+      </c>
+      <c r="F140" s="1">
+        <v>0</v>
+      </c>
       <c r="G140" s="1"/>
       <c r="H140" s="1"/>
       <c r="I140" s="1"/>

</xml_diff>